<commit_message>
add data driven for tcs ingteration test
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,24 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1616D6B4-CDE9-42FC-B7BF-25EC46763B1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23226E14-CC80-46F3-81F6-73A17EF2B90E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="FPA 001" sheetId="4" r:id="rId1"/>
-    <sheet name="FPA 002-003-005-007" sheetId="6" r:id="rId2"/>
-    <sheet name="FPA 004-006" sheetId="7" r:id="rId3"/>
-    <sheet name="FPA 008-009" sheetId="5" r:id="rId4"/>
+    <sheet name="FPA001" sheetId="4" r:id="rId1"/>
+    <sheet name="FPA002-003-005-007" sheetId="6" r:id="rId2"/>
+    <sheet name="FPA004-006-010" sheetId="7" r:id="rId3"/>
+    <sheet name="FPA008-009" sheetId="5" r:id="rId4"/>
     <sheet name="BTMI003" sheetId="10" r:id="rId5"/>
     <sheet name="BTMI015" sheetId="9" r:id="rId6"/>
+    <sheet name="Calculate" sheetId="11" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'FPA008-009'!$A$1:$Q$4</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="64">
   <si>
     <t>fileName</t>
   </si>
@@ -72,15 +76,6 @@
     <t>packagingAndShippingComments</t>
   </si>
   <si>
-    <t>auto_Milling.step</t>
-  </si>
-  <si>
-    <t>goCAD_milling v4.pdf</t>
-  </si>
-  <si>
-    <t>Eloxieren</t>
-  </si>
-  <si>
     <t>Ra 0,8 - 1,6 (finely finished); Rz 6,3 - 10</t>
   </si>
   <si>
@@ -111,9 +106,6 @@
     <t>customerEmail</t>
   </si>
   <si>
-    <t>truongbaothuy93@gmail.com</t>
-  </si>
-  <si>
     <t>step-testing.step</t>
   </si>
   <si>
@@ -193,6 +185,42 @@
   </si>
   <si>
     <t>392,41</t>
+  </si>
+  <si>
+    <t>58,04</t>
+  </si>
+  <si>
+    <t>ECONOMY</t>
+  </si>
+  <si>
+    <t>Pickup at factory</t>
+  </si>
+  <si>
+    <t>stp-testing 3.stp</t>
+  </si>
+  <si>
+    <t>FAST</t>
+  </si>
+  <si>
+    <t>Special packaging / via freight forwarding</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Add Months</t>
+  </si>
+  <si>
+    <t>Date M added</t>
+  </si>
+  <si>
+    <t>step-testing 2.step</t>
+  </si>
+  <si>
+    <t>buyer@gocad.de</t>
   </si>
 </sst>
 </file>
@@ -256,7 +284,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -280,6 +308,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -556,10 +596,647 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="3" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="4">
+        <v>5</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="4">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="4">
+        <v>7</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC3FC65-E1BB-4B27-9BAD-1FAD73694C2F}">
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="18.85546875" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" customWidth="1"/>
+    <col min="16" max="16" width="31.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="3" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4">
+        <v>150</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="4">
+        <v>5</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4">
+        <v>50</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="4">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4">
+        <v>100</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="4">
+        <v>7</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E9DDA8-B5FB-4116-AA3C-6DFE9FE54EE5}">
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="3" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="4">
+        <v>5</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="4">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="4">
+        <v>7</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08C9849-CB54-465E-AADF-08DB0E1F7827}">
+  <dimension ref="A1:Q4"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -573,408 +1250,10 @@
     <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1"/>
-    <col min="16" max="16" width="31.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="4">
-        <v>5</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="5">
-        <v>45276</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC3FC65-E1BB-4B27-9BAD-1FAD73694C2F}">
-  <dimension ref="A1:P2"/>
-  <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:BE1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1"/>
-    <col min="16" max="16" width="31.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4">
-        <v>150</v>
-      </c>
-      <c r="D2" s="4">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="4">
-        <v>5</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="5">
-        <v>45276</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E9DDA8-B5FB-4116-AA3C-6DFE9FE54EE5}">
-  <dimension ref="A1:P2"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1"/>
-    <col min="16" max="16" width="31.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="4">
-        <v>5</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="5">
-        <v>45276</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08C9849-CB54-465E-AADF-08DB0E1F7827}">
-  <dimension ref="A1:Q2"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1"/>
+    <col min="11" max="12" width="18.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1014,33 +1293,31 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B2" s="4"/>
       <c r="C2" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="4">
         <v>3</v>
@@ -1049,40 +1326,145 @@
         <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H2" s="4">
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="5">
+        <f ca="1">Calculate!$C$2</f>
+        <v>45349</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="5">
-        <v>45276</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="Q2" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>28</v>
+      </c>
+      <c r="H3" s="4">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="5">
+        <f ca="1">Calculate!$C$2</f>
+        <v>45349</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="4">
+        <v>7</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="5">
+        <f ca="1">Calculate!$C$2</f>
+        <v>45349</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1094,8 +1476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504AB99D-61BC-4A19-95BC-D98B671BEA2F}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1150,15 +1532,15 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
@@ -1171,33 +1553,33 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H2" s="4">
         <v>4</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1210,28 +1592,28 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1243,8 +1625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247EA267-3747-4ADE-8941-713003159070}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M1" sqref="A1:M1048576"/>
+    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1307,39 +1689,39 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="U1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:21">
       <c r="A2" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
@@ -1352,28 +1734,28 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H2" s="4">
         <v>4</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="N2" s="4">
         <v>2</v>
@@ -1385,24 +1767,24 @@
         <v>6</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1415,28 +1797,28 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="N3" s="4">
         <v>1</v>
@@ -1448,20 +1830,66 @@
         <v>6</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="S3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="T3" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>53</v>
-      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA620B2-AF97-4CF6-81E1-3C974CAF77F3}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="10">
+        <f ca="1">TODAY()</f>
+        <v>45196</v>
+      </c>
+      <c r="B2" s="9">
+        <v>5</v>
+      </c>
+      <c r="C2" s="11">
+        <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
+        <v>45349</v>
+      </c>
+      <c r="D2" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix bug BTMI tcs
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE61D235-2DE1-4A62-AB0D-925E1004CA53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920F0E92-CA12-4F91-B9AC-589D7132CC69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="63">
   <si>
     <t>fileName</t>
   </si>
@@ -172,15 +172,9 @@
     <t>stp-testing 2.stp</t>
   </si>
   <si>
-    <t>342,45</t>
-  </si>
-  <si>
     <t>234,69</t>
   </si>
   <si>
-    <t>998,63</t>
-  </si>
-  <si>
     <t>151,02</t>
   </si>
   <si>
@@ -220,10 +214,10 @@
     <t>buyer@gocad.de</t>
   </si>
   <si>
-    <t>391,90</t>
-  </si>
-  <si>
-    <t>239,95</t>
+    <t>341,94</t>
+  </si>
+  <si>
+    <t>998,12</t>
   </si>
 </sst>
 </file>
@@ -744,15 +738,15 @@
         <v>41</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -786,10 +780,10 @@
         <v>38</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -958,13 +952,13 @@
         <v>41</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>21</v>
@@ -972,7 +966,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1006,13 +1000,13 @@
         <v>38</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>21</v>
@@ -1118,7 +1112,7 @@
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>17</v>
@@ -1163,7 +1157,7 @@
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>17</v>
@@ -1175,18 +1169,18 @@
         <v>41</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1208,7 +1202,7 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>17</v>
@@ -1220,13 +1214,13 @@
         <v>38</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1351,7 +1345,7 @@
       </c>
       <c r="M2" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45353</v>
+        <v>45354</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>19</v>
@@ -1363,7 +1357,7 @@
         <v>21</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1403,24 +1397,24 @@
       </c>
       <c r="M3" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45353</v>
+        <v>45354</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>21</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1455,19 +1449,19 @@
       </c>
       <c r="M4" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45353</v>
+        <v>45354</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1480,7 +1474,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1577,7 +1571,7 @@
         <v>38</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1616,7 +1610,7 @@
         <v>41</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1628,8 +1622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247EA267-3747-4ADE-8941-713003159070}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1758,7 +1752,7 @@
         <v>38</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="N2" s="4">
         <v>2</v>
@@ -1782,7 +1776,7 @@
         <v>41</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -1821,7 +1815,7 @@
         <v>41</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="N3" s="4">
         <v>1</v>
@@ -1845,7 +1839,7 @@
         <v>38</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1871,26 +1865,26 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45201</v>
+        <v>45202</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45353</v>
+        <v>45354</v>
       </c>
       <c r="D2" s="8"/>
     </row>

</xml_diff>

<commit_message>
add content manual for buyer
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920F0E92-CA12-4F91-B9AC-589D7132CC69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B0B6DB-C6B6-4C69-80E9-1CDE50EC61D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA001" sheetId="4" r:id="rId1"/>
     <sheet name="FPA002-003-005-007" sheetId="6" r:id="rId2"/>
     <sheet name="FPA004-006-010" sheetId="7" r:id="rId3"/>
     <sheet name="FPA008-009" sheetId="5" r:id="rId4"/>
-    <sheet name="BTMI003" sheetId="10" r:id="rId5"/>
-    <sheet name="BTMI015" sheetId="9" r:id="rId6"/>
-    <sheet name="Calculate" sheetId="11" r:id="rId7"/>
+    <sheet name="BTMI002" sheetId="12" r:id="rId5"/>
+    <sheet name="BTMI003" sheetId="10" r:id="rId6"/>
+    <sheet name="BTMI015" sheetId="9" r:id="rId7"/>
+    <sheet name="Calculate" sheetId="11" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'FPA008-009'!$A$1:$Q$4</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="71">
   <si>
     <t>fileName</t>
   </si>
@@ -218,6 +219,30 @@
   </si>
   <si>
     <t>998,12</t>
+  </si>
+  <si>
+    <t>codeManual</t>
+  </si>
+  <si>
+    <t>SYSTEM_ERROR</t>
+  </si>
+  <si>
+    <t>CANNOT_CALCULATE_PART</t>
+  </si>
+  <si>
+    <t>PRICE_EXCEED_THRESHOLD</t>
+  </si>
+  <si>
+    <t>SMALL_TOLERANCES</t>
+  </si>
+  <si>
+    <t>CANNOT_MANUFACTURE_PART</t>
+  </si>
+  <si>
+    <t>CALCULATION_ERROR</t>
+  </si>
+  <si>
+    <t>stp-testing.stp</t>
   </si>
 </sst>
 </file>
@@ -281,7 +306,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -317,6 +342,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1470,11 +1498,316 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544CF78C-E801-4C61-A3AF-6B74429A6B71}">
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="4">
+        <v>4</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12">
+        <v>1</v>
+      </c>
+      <c r="E3" s="12">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="4">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4">
+        <v>300</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="4">
+        <v>7</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4">
+        <v>300</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="4">
+        <v>7</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4">
+        <v>300</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="4">
+        <v>7</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4">
+        <v>300</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>3</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="4">
+        <v>7</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504AB99D-61BC-4A19-95BC-D98B671BEA2F}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1618,11 +1951,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247EA267-3747-4ADE-8941-713003159070}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
@@ -1847,7 +2180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA620B2-AF97-4CF6-81E1-3C974CAF77F3}">
   <dimension ref="A1:D2"/>
   <sheetViews>

</xml_diff>

<commit_message>
fix value data driven
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EC9C80-FB33-4DFF-9174-3D59D1A70213}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C938AFD-2AD7-49DB-84AB-F0F588DE7894}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA001" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="71">
   <si>
     <t>fileName</t>
   </si>
@@ -173,12 +173,6 @@
     <t>stp-testing 2.stp</t>
   </si>
   <si>
-    <t>234,69</t>
-  </si>
-  <si>
-    <t>151,02</t>
-  </si>
-  <si>
     <t>58,04</t>
   </si>
   <si>
@@ -215,12 +209,6 @@
     <t>buyer@gocad.de</t>
   </si>
   <si>
-    <t>341,94</t>
-  </si>
-  <si>
-    <t>998,12</t>
-  </si>
-  <si>
     <t>codeManual</t>
   </si>
   <si>
@@ -249,6 +237,12 @@
   </si>
   <si>
     <t>359,94</t>
+  </si>
+  <si>
+    <t>158,97</t>
+  </si>
+  <si>
+    <t>1.050,66</t>
   </si>
 </sst>
 </file>
@@ -772,15 +766,15 @@
         <v>41</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -814,10 +808,10 @@
         <v>38</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -986,13 +980,13 @@
         <v>41</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>21</v>
@@ -1000,7 +994,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1034,13 +1028,13 @@
         <v>38</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>21</v>
@@ -1146,7 +1140,7 @@
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>17</v>
@@ -1191,7 +1185,7 @@
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>17</v>
@@ -1203,18 +1197,18 @@
         <v>41</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1236,7 +1230,7 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>17</v>
@@ -1248,13 +1242,13 @@
         <v>38</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1379,7 +1373,7 @@
       </c>
       <c r="M2" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45354</v>
+        <v>45361</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>19</v>
@@ -1391,7 +1385,7 @@
         <v>21</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1431,24 +1425,24 @@
       </c>
       <c r="M3" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45354</v>
+        <v>45361</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>21</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1483,19 +1477,19 @@
       </c>
       <c r="M4" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45354</v>
+        <v>45361</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1566,7 +1560,7 @@
         <v>29</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1593,7 +1587,7 @@
         <v>4</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>17</v>
@@ -1605,12 +1599,12 @@
         <v>38</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12">
@@ -1644,12 +1638,12 @@
         <v>38</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1683,12 +1677,12 @@
         <v>38</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4">
@@ -1722,12 +1716,12 @@
         <v>38</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4">
@@ -1761,12 +1755,12 @@
         <v>38</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4">
@@ -1800,7 +1794,7 @@
         <v>38</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1812,7 +1806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504AB99D-61BC-4A19-95BC-D98B671BEA2F}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
@@ -1910,7 +1904,7 @@
         <v>38</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1949,7 +1943,7 @@
         <v>41</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1961,8 +1955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247EA267-3747-4ADE-8941-713003159070}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2091,7 +2085,7 @@
         <v>38</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="N2" s="4">
         <v>2</v>
@@ -2115,7 +2109,7 @@
         <v>41</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -2154,7 +2148,7 @@
         <v>41</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="N3" s="4">
         <v>1</v>
@@ -2178,7 +2172,7 @@
         <v>38</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2204,26 +2198,26 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45202</v>
+        <v>45209</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45354</v>
+        <v>45361</v>
       </c>
       <c r="D2" s="8"/>
     </row>

</xml_diff>

<commit_message>
fix bug deburring field change UI
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C938AFD-2AD7-49DB-84AB-F0F588DE7894}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E48333-F610-4FF6-909D-F165B266A6D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA001" sheetId="4" r:id="rId1"/>
@@ -824,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC3FC65-E1BB-4B27-9BAD-1FAD73694C2F}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -902,7 +902,7 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="D2" s="4">
         <v>3</v>
@@ -998,7 +998,7 @@
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -1373,7 +1373,7 @@
       </c>
       <c r="M2" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45361</v>
+        <v>45368</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>19</v>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="M3" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45361</v>
+        <v>45368</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>48</v>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="M4" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45361</v>
+        <v>45368</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>51</v>
@@ -1955,7 +1955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247EA267-3747-4ADE-8941-713003159070}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
@@ -2210,14 +2210,14 @@
     <row r="2" spans="1:4">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45209</v>
+        <v>45216</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45361</v>
+        <v>45368</v>
       </c>
       <c r="D2" s="8"/>
     </row>

</xml_diff>

<commit_message>
fix some cases SMP
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE615B88-EAB9-4C69-854E-D4A7B4DCFFCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F62F845-D2C2-4AA9-8B5A-DBCF1E1B95E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA001" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="80">
   <si>
     <t>fileName</t>
   </si>
@@ -258,6 +258,18 @@
   </si>
   <si>
     <t>Soft annealing</t>
+  </si>
+  <si>
+    <t>X5CrNi18</t>
+  </si>
+  <si>
+    <t>EN AW-6060 / AlMgSi</t>
+  </si>
+  <si>
+    <t>materialGroupChanged</t>
+  </si>
+  <si>
+    <t>TECATRON / PPS</t>
   </si>
 </sst>
 </file>
@@ -1277,7 +1289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08C9849-CB54-465E-AADF-08DB0E1F7827}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
@@ -1390,7 +1402,7 @@
       </c>
       <c r="M2" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45425</v>
+        <v>45426</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>18</v>
@@ -1442,7 +1454,7 @@
       </c>
       <c r="M3" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45425</v>
+        <v>45426</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>47</v>
@@ -1494,7 +1506,7 @@
       </c>
       <c r="M4" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45425</v>
+        <v>45426</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>50</v>
@@ -1970,10 +1982,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247EA267-3747-4ADE-8941-713003159070}">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1988,7 +2000,7 @@
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
     <col min="12" max="12" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.7109375" customWidth="1"/>
     <col min="14" max="14" width="26.85546875" bestFit="1" customWidth="1"/>
@@ -1996,12 +2008,13 @@
     <col min="16" max="16" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="33" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="3" customFormat="1">
+    <row r="1" spans="1:22" s="3" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2057,16 +2070,19 @@
         <v>34</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
         <v>24</v>
       </c>
@@ -2093,10 +2109,10 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>37</v>
@@ -2120,16 +2136,19 @@
         <v>26</v>
       </c>
       <c r="S2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="U2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:22">
       <c r="A3" s="4" t="s">
         <v>45</v>
       </c>
@@ -2156,10 +2175,10 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>40</v>
@@ -2183,12 +2202,15 @@
         <v>15</v>
       </c>
       <c r="S3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="T3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="U3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="V3" s="4" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2227,14 +2249,14 @@
     <row r="2" spans="1:4">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45273</v>
+        <v>45274</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45425</v>
+        <v>45426</v>
       </c>
       <c r="D2" s="8"/>
     </row>

</xml_diff>

<commit_message>
fix change value customer email
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783D6BF2-2B75-41EC-8045-38F38FE38B82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D827FB6-FF45-4A38-B54B-6B8B889F46D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA001" sheetId="4" r:id="rId1"/>
@@ -194,9 +194,6 @@
     <t>step-testing 2.step</t>
   </si>
   <si>
-    <t>buyer@gocad.de</t>
-  </si>
-  <si>
     <t>codeManual</t>
   </si>
   <si>
@@ -273,6 +270,9 @@
   </si>
   <si>
     <t>664,15</t>
+  </si>
+  <si>
+    <t>thuyautomation0@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -653,7 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E21" sqref="E21:F21"/>
     </sheetView>
   </sheetViews>
@@ -745,7 +745,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -775,7 +775,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>27</v>
@@ -787,10 +787,10 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>40</v>
@@ -804,7 +804,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -829,7 +829,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -953,7 +953,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -989,7 +989,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>27</v>
@@ -1001,10 +1001,10 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>40</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1049,7 +1049,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -1175,7 +1175,7 @@
         <v>49</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1220,7 +1220,7 @@
         <v>49</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>41</v>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1265,7 +1265,7 @@
         <v>49</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -1292,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08C9849-CB54-465E-AADF-08DB0E1F7827}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1395,7 +1395,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="M2" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45430</v>
+        <v>45438</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>18</v>
@@ -1417,7 +1417,7 @@
         <v>20</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1435,7 +1435,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>27</v>
@@ -1447,17 +1447,17 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>40</v>
       </c>
       <c r="M3" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45430</v>
+        <v>45438</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>45</v>
@@ -1469,12 +1469,12 @@
         <v>20</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1499,7 +1499,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="M4" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45430</v>
+        <v>45438</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>47</v>
@@ -1521,7 +1521,7 @@
         <v>20</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1592,7 +1592,7 @@
         <v>28</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1622,7 +1622,7 @@
         <v>49</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1631,12 +1631,12 @@
         <v>37</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12">
@@ -1661,7 +1661,7 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>39</v>
@@ -1670,7 +1670,7 @@
         <v>37</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1700,7 +1700,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -1709,12 +1709,12 @@
         <v>37</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4">
@@ -1739,7 +1739,7 @@
         <v>16</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>39</v>
@@ -1748,7 +1748,7 @@
         <v>37</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1778,7 +1778,7 @@
         <v>16</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>39</v>
@@ -1787,7 +1787,7 @@
         <v>37</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1817,7 +1817,7 @@
         <v>16</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>39</v>
@@ -1826,7 +1826,7 @@
         <v>37</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1927,7 +1927,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1936,7 +1936,7 @@
         <v>37</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1966,7 +1966,7 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>41</v>
@@ -1975,7 +1975,7 @@
         <v>40</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2073,7 +2073,7 @@
         <v>34</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>35</v>
@@ -2100,7 +2100,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>15</v>
@@ -2112,16 +2112,16 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>37</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N2" s="4">
         <v>2</v>
@@ -2139,7 +2139,7 @@
         <v>26</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>39</v>
@@ -2148,7 +2148,7 @@
         <v>40</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -2178,16 +2178,16 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>40</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N3" s="4">
         <v>1</v>
@@ -2199,22 +2199,22 @@
         <v>6</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="U3" s="7" t="s">
         <v>37</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2252,14 +2252,14 @@
     <row r="2" spans="1:4">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45278</v>
+        <v>45286</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45430</v>
+        <v>45438</v>
       </c>
       <c r="D2" s="8"/>
     </row>

</xml_diff>

<commit_message>
add data driven for error calculation
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D827FB6-FF45-4A38-B54B-6B8B889F46D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485C2F05-DAC0-4973-B9A2-3A4BAA03B7E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA001" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="78">
   <si>
     <t>fileName</t>
   </si>
@@ -197,19 +197,10 @@
     <t>codeManual</t>
   </si>
   <si>
-    <t>SYSTEM_ERROR</t>
-  </si>
-  <si>
-    <t>CANNOT_CALCULATE_PART</t>
-  </si>
-  <si>
     <t>PRICE_EXCEED_THRESHOLD</t>
   </si>
   <si>
     <t>SMALL_TOLERANCES</t>
-  </si>
-  <si>
-    <t>CANNOT_MANUFACTURE_PART</t>
   </si>
   <si>
     <t>CALCULATION_ERROR</t>
@@ -745,7 +736,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -775,7 +766,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>27</v>
@@ -787,10 +778,10 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>40</v>
@@ -804,7 +795,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -829,7 +820,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -953,7 +944,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -989,7 +980,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>27</v>
@@ -1001,10 +992,10 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>40</v>
@@ -1024,7 +1015,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1049,7 +1040,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -1175,7 +1166,7 @@
         <v>49</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1220,7 +1211,7 @@
         <v>49</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>41</v>
@@ -1240,7 +1231,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1265,7 +1256,7 @@
         <v>49</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -1292,7 +1283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08C9849-CB54-465E-AADF-08DB0E1F7827}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
@@ -1395,7 +1386,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1417,7 +1408,7 @@
         <v>20</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1435,7 +1426,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>27</v>
@@ -1447,10 +1438,10 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>40</v>
@@ -1469,12 +1460,12 @@
         <v>20</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1499,7 +1490,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -1521,7 +1512,7 @@
         <v>20</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1531,11 +1522,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544CF78C-E801-4C61-A3AF-6B74429A6B71}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1622,7 +1611,7 @@
         <v>49</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1631,25 +1620,25 @@
         <v>37</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D3" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>27</v>
@@ -1661,7 +1650,7 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>39</v>
@@ -1670,7 +1659,7 @@
         <v>37</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1678,17 +1667,17 @@
         <v>53</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="4">
-        <v>300</v>
-      </c>
-      <c r="D4" s="4">
-        <v>2</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="C4" s="12">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="12">
+        <v>2</v>
+      </c>
+      <c r="E4" s="12">
         <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>27</v>
@@ -1700,7 +1689,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -1709,124 +1698,7 @@
         <v>37</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4">
-        <v>300</v>
-      </c>
-      <c r="D5" s="4">
-        <v>2</v>
-      </c>
-      <c r="E5" s="4">
-        <v>3</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="4">
-        <v>7</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4">
-        <v>300</v>
-      </c>
-      <c r="D6" s="4">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4">
-        <v>3</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="4">
-        <v>7</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" s="4" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4">
-        <v>300</v>
-      </c>
-      <c r="D7" s="4">
-        <v>2</v>
-      </c>
-      <c r="E7" s="4">
-        <v>3</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="4">
-        <v>7</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1927,7 +1799,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1936,7 +1808,7 @@
         <v>37</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1966,7 +1838,7 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>41</v>
@@ -1975,7 +1847,7 @@
         <v>40</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2073,7 +1945,7 @@
         <v>34</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>35</v>
@@ -2100,7 +1972,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>15</v>
@@ -2112,16 +1984,16 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>37</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="N2" s="4">
         <v>2</v>
@@ -2139,7 +2011,7 @@
         <v>26</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>39</v>
@@ -2148,7 +2020,7 @@
         <v>40</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -2178,16 +2050,16 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>40</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N3" s="4">
         <v>1</v>
@@ -2199,22 +2071,22 @@
         <v>6</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="R3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="U3" s="7" t="s">
         <v>37</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change adapt GM site
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485C2F05-DAC0-4973-B9A2-3A4BAA03B7E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A17732-2202-4E6A-AD8F-911E518CE1BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA001" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="84">
   <si>
     <t>fileName</t>
   </si>
@@ -264,6 +264,24 @@
   </si>
   <si>
     <t>thuyautomation0@gmail.com</t>
+  </si>
+  <si>
+    <t>Rubber</t>
+  </si>
+  <si>
+    <t>Moosgummi EPDM (schwarz)</t>
+  </si>
+  <si>
+    <t>SBR 40 (grau)</t>
+  </si>
+  <si>
+    <t>Plastic</t>
+  </si>
+  <si>
+    <t>compliances</t>
+  </si>
+  <si>
+    <t>PEEK GF (natur - beige)</t>
   </si>
 </sst>
 </file>
@@ -642,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:F21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -657,15 +675,14 @@
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.5703125" customWidth="1"/>
     <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="27.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1">
+    <row r="1" spans="1:13" s="3" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -682,7 +699,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -691,25 +708,22 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
         <v>24</v>
       </c>
@@ -723,9 +737,7 @@
       <c r="E2" s="4">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
@@ -733,25 +745,22 @@
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>37</v>
       </c>
+      <c r="L2" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="M2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -765,9 +774,7 @@
       <c r="E3" s="4">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
         <v>27</v>
       </c>
@@ -775,25 +782,22 @@
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="L3" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>40</v>
       </c>
+      <c r="L3" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="M3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
         <v>71</v>
       </c>
@@ -807,9 +811,7 @@
       <c r="E4" s="4">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
         <v>26</v>
       </c>
@@ -817,21 +819,18 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="7" t="s">
         <v>37</v>
       </c>
+      <c r="L4" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="M4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -843,10 +842,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC3FC65-E1BB-4B27-9BAD-1FAD73694C2F}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -858,16 +857,15 @@
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" customWidth="1"/>
     <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" customWidth="1"/>
-    <col min="11" max="12" width="18.85546875" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1"/>
-    <col min="16" max="16" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" customWidth="1"/>
+    <col min="10" max="11" width="18.85546875" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" customWidth="1"/>
+    <col min="15" max="15" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1">
+    <row r="1" spans="1:15" s="3" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -893,31 +891,28 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:15">
       <c r="A2" s="4" t="s">
         <v>24</v>
       </c>
@@ -941,31 +936,28 @@
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>37</v>
       </c>
+      <c r="L2" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="M2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:15">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -989,31 +981,28 @@
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>40</v>
       </c>
+      <c r="L3" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="M3" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="P3" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:15">
       <c r="A4" s="4" t="s">
         <v>71</v>
       </c>
@@ -1037,27 +1026,24 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>37</v>
       </c>
+      <c r="L4" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="M4" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="P4" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1396,7 +1382,7 @@
       </c>
       <c r="M2" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45438</v>
+        <v>45447</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>18</v>
@@ -1448,7 +1434,7 @@
       </c>
       <c r="M3" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45438</v>
+        <v>45447</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>45</v>
@@ -1500,7 +1486,7 @@
       </c>
       <c r="M4" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45438</v>
+        <v>45447</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>47</v>
@@ -1524,7 +1510,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544CF78C-E801-4C61-A3AF-6B74429A6B71}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2124,14 +2112,14 @@
     <row r="2" spans="1:4">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45286</v>
+        <v>45295</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45438</v>
+        <v>45447</v>
       </c>
       <c r="D2" s="8"/>
     </row>

</xml_diff>

<commit_message>
change add compliances field
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A17732-2202-4E6A-AD8F-911E518CE1BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DD851C-FA8D-4EA7-9A5C-75AFC66D5879}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA001" sheetId="4" r:id="rId1"/>
@@ -23,14 +23,14 @@
     <sheet name="Calculate" sheetId="11" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'FPA008-009'!$A$1:$Q$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'FPA008-009'!$A$1:$P$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="66">
   <si>
     <t>fileName</t>
   </si>
@@ -47,9 +47,6 @@
     <t>tolerancesNum</t>
   </si>
   <si>
-    <t>surfaceTreatment</t>
-  </si>
-  <si>
     <t>quality</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>EN AW-7075 / AlZn5</t>
-  </si>
-  <si>
     <t>STANDARD</t>
   </si>
   <si>
@@ -107,9 +101,6 @@
     <t>step-testing.step</t>
   </si>
   <si>
-    <t>Sandblasting</t>
-  </si>
-  <si>
     <t>Ra 3,2 - 25 (roughed); Rz 16 - 100</t>
   </si>
   <si>
@@ -131,9 +122,6 @@
     <t>tolerancesNumChanged</t>
   </si>
   <si>
-    <t>surfaceTreatmentChanged</t>
-  </si>
-  <si>
     <t>qualityChanged</t>
   </si>
   <si>
@@ -146,21 +134,9 @@
     <t>false</t>
   </si>
   <si>
-    <t>Grinding</t>
-  </si>
-  <si>
-    <t>TECAFLON PTFE natural</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
-    <t>TECAST L black</t>
-  </si>
-  <si>
-    <t>Glass bead blasting</t>
-  </si>
-  <si>
     <t>stp-testing 2.stp</t>
   </si>
   <si>
@@ -179,9 +155,6 @@
     <t>Special packaging / via freight forwarding</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -215,30 +188,6 @@
     <t>359,94</t>
   </si>
   <si>
-    <t>Aluminum</t>
-  </si>
-  <si>
-    <t>PA 6 C</t>
-  </si>
-  <si>
-    <t>TECAFLON / PTFE, PVDF</t>
-  </si>
-  <si>
-    <t>X2CrNiMo17</t>
-  </si>
-  <si>
-    <t>Stainless steel</t>
-  </si>
-  <si>
-    <t>Soft annealing</t>
-  </si>
-  <si>
-    <t>X5CrNi18</t>
-  </si>
-  <si>
-    <t>EN AW-6060 / AlMgSi</t>
-  </si>
-  <si>
     <t>materialGroupChanged</t>
   </si>
   <si>
@@ -251,15 +200,9 @@
     <t>183,38</t>
   </si>
   <si>
-    <t>EN AW-6082 / AlMgSi1</t>
-  </si>
-  <si>
     <t>96,54</t>
   </si>
   <si>
-    <t>Phosphating</t>
-  </si>
-  <si>
     <t>664,15</t>
   </si>
   <si>
@@ -282,6 +225,9 @@
   </si>
   <si>
     <t>PEEK GF (natur - beige)</t>
+  </si>
+  <si>
+    <t>compliancesChanged</t>
   </si>
 </sst>
 </file>
@@ -662,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -699,33 +645,33 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
@@ -739,30 +685,30 @@
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="4">
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -776,30 +722,30 @@
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -813,25 +759,25 @@
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H4" s="4">
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -845,7 +791,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -882,39 +828,39 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
@@ -926,40 +872,38 @@
       <c r="E2" s="4">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="4">
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="4" t="s">
+      <c r="N2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -971,40 +915,38 @@
       <c r="E3" s="4">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="4" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1016,35 +958,33 @@
       <c r="E4" s="4">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H4" s="4">
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="M4" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1054,10 +994,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E9DDA8-B5FB-4116-AA3C-6DFE9FE54EE5}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="I2" sqref="I2:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1069,16 +1009,15 @@
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1">
+    <row r="1" spans="1:14" s="3" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1095,13 +1034,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
@@ -1110,24 +1049,21 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
@@ -1139,40 +1075,35 @@
       <c r="E2" s="4">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="4">
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="N2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1184,40 +1115,35 @@
       <c r="E3" s="4">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>40</v>
+        <v>60</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1229,35 +1155,30 @@
       <c r="E4" s="4">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H4" s="4">
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>37</v>
-      </c>
       <c r="M4" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1267,10 +1188,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08C9849-CB54-465E-AADF-08DB0E1F7827}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1282,17 +1203,16 @@
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18.85546875" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1">
+    <row r="1" spans="1:16" s="3" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1309,13 +1229,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
@@ -1324,10 +1244,10 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>11</v>
@@ -1335,19 +1255,16 @@
       <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
@@ -1359,47 +1276,42 @@
       <c r="E2" s="4">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="4">
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="5">
+        <v>64</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="5">
         <f ca="1">Calculate!$C$2</f>
         <v>45447</v>
       </c>
+      <c r="M2" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="N2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="P2" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1411,47 +1323,42 @@
       <c r="E3" s="4">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="M3" s="5">
+        <v>60</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="5">
         <f ca="1">Calculate!$C$2</f>
         <v>45447</v>
       </c>
+      <c r="M3" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="N3" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+        <v>18</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="4" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1463,42 +1370,37 @@
       <c r="E4" s="4">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H4" s="4">
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" s="5">
+        <v>61</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="5">
         <f ca="1">Calculate!$C$2</f>
         <v>45447</v>
       </c>
+      <c r="M4" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="N4" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>77</v>
+        <v>18</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1508,10 +1410,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544CF78C-E801-4C61-A3AF-6B74429A6B71}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="I2" sqref="I2:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1524,14 +1426,13 @@
     <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1548,13 +1449,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
@@ -1563,18 +1464,15 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
@@ -1586,34 +1484,29 @@
       <c r="E2" s="4">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="4">
         <v>4</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12">
@@ -1625,34 +1518,29 @@
       <c r="E3" s="12">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>60</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="4" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="12">
@@ -1664,29 +1552,24 @@
       <c r="E4" s="12">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H4" s="4">
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1699,7 +1582,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J2" sqref="J2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1712,7 +1595,7 @@
     <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.5703125" bestFit="1" customWidth="1"/>
@@ -1736,33 +1619,33 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
@@ -1774,34 +1657,32 @@
       <c r="E2" s="4">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="4">
         <v>4</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1813,29 +1694,27 @@
       <c r="E3" s="4">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1847,8 +1726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247EA267-3747-4ADE-8941-713003159070}">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1894,60 +1773,60 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="V1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
@@ -1959,29 +1838,27 @@
       <c r="E2" s="4">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="4">
         <v>4</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="N2" s="4">
         <v>2</v>
@@ -1992,28 +1869,26 @@
       <c r="P2" s="4">
         <v>6</v>
       </c>
-      <c r="Q2" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="Q2" s="4"/>
       <c r="R2" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -2025,29 +1900,27 @@
       <c r="E3" s="4">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="N3" s="4">
         <v>1</v>
@@ -2058,23 +1931,21 @@
       <c r="P3" s="4">
         <v>6</v>
       </c>
-      <c r="Q3" s="4" t="s">
-        <v>75</v>
-      </c>
+      <c r="Q3" s="4"/>
       <c r="R3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="T3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="T3" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="U3" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2100,13 +1971,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="9" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>

<commit_message>
change name material group
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485C2F05-DAC0-4973-B9A2-3A4BAA03B7E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CE68C3-E86A-4727-B935-E928704B4237}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,9 +215,6 @@
     <t>359,94</t>
   </si>
   <si>
-    <t>Aluminum</t>
-  </si>
-  <si>
     <t>PA 6 C</t>
   </si>
   <si>
@@ -264,6 +261,9 @@
   </si>
   <si>
     <t>thuyautomation0@gmail.com</t>
+  </si>
+  <si>
+    <t>Aluminium</t>
   </si>
 </sst>
 </file>
@@ -736,7 +736,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -766,7 +766,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>27</v>
@@ -778,10 +778,10 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>40</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -820,7 +820,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -944,7 +944,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -980,7 +980,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>27</v>
@@ -992,10 +992,10 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>40</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1040,7 +1040,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -1166,7 +1166,7 @@
         <v>49</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1211,7 +1211,7 @@
         <v>49</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>41</v>
@@ -1231,7 +1231,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1256,7 +1256,7 @@
         <v>49</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -1386,7 +1386,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="M2" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45438</v>
+        <v>45449</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>18</v>
@@ -1408,7 +1408,7 @@
         <v>20</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1426,7 +1426,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>27</v>
@@ -1438,17 +1438,17 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>40</v>
       </c>
       <c r="M3" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45438</v>
+        <v>45449</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>45</v>
@@ -1460,12 +1460,12 @@
         <v>20</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1490,7 +1490,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -1500,7 +1500,7 @@
       </c>
       <c r="M4" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45438</v>
+        <v>45449</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>47</v>
@@ -1512,7 +1512,7 @@
         <v>20</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1524,7 +1524,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544CF78C-E801-4C61-A3AF-6B74429A6B71}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1611,7 +1613,7 @@
         <v>49</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1650,7 +1652,7 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>39</v>
@@ -1689,7 +1691,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>39</v>
@@ -1799,7 +1801,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1838,7 +1840,7 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>41</v>
@@ -1945,7 +1947,7 @@
         <v>34</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>35</v>
@@ -1972,7 +1974,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>15</v>
@@ -1984,16 +1986,16 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>37</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N2" s="4">
         <v>2</v>
@@ -2011,7 +2013,7 @@
         <v>26</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>39</v>
@@ -2020,7 +2022,7 @@
         <v>40</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -2050,16 +2052,16 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>40</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N3" s="4">
         <v>1</v>
@@ -2071,22 +2073,22 @@
         <v>6</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U3" s="7" t="s">
         <v>37</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2124,14 +2126,14 @@
     <row r="2" spans="1:4">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45286</v>
+        <v>45297</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45438</v>
+        <v>45449</v>
       </c>
       <c r="D2" s="8"/>
     </row>

</xml_diff>

<commit_message>
fix change data driven
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2032F19-E9DC-4B15-BD95-A9E83BC4E97C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A008A0-6B1D-4A8E-BE28-9EB1139251DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA001" sheetId="4" r:id="rId1"/>
@@ -206,9 +206,6 @@
     <t>Edit compliances</t>
   </si>
   <si>
-    <t>stp-testing 3.stp</t>
-  </si>
-  <si>
     <t>TECADUR / PBT</t>
   </si>
   <si>
@@ -228,6 +225,9 @@
   </si>
   <si>
     <t>ipt-testing.ipt</t>
+  </si>
+  <si>
+    <t>stp-testing 4.stp</t>
   </si>
 </sst>
 </file>
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -691,10 +691,10 @@
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>33</v>
@@ -708,7 +708,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -728,10 +728,10 @@
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>34</v>
@@ -745,7 +745,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -765,10 +765,10 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>33</v>
@@ -791,7 +791,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -880,10 +880,10 @@
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>33</v>
@@ -903,7 +903,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -923,10 +923,10 @@
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>34</v>
@@ -946,7 +946,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -966,10 +966,10 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>33</v>
@@ -996,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E9DDA8-B5FB-4116-AA3C-6DFE9FE54EE5}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1085,10 +1085,10 @@
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>33</v>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1127,10 +1127,10 @@
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>34</v>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1169,10 +1169,10 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>33</v>
@@ -1197,7 +1197,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1290,17 +1290,17 @@
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>33</v>
       </c>
       <c r="L2" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45454</v>
+        <v>45455</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>16</v>
@@ -1317,7 +1317,7 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1337,17 +1337,17 @@
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>34</v>
       </c>
       <c r="L3" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45454</v>
+        <v>45455</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>36</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1384,17 +1384,17 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>33</v>
       </c>
       <c r="L4" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45454</v>
+        <v>45455</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>38</v>
@@ -1498,10 +1498,10 @@
         <v>4</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>33</v>
@@ -1512,7 +1512,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12">
@@ -1532,10 +1532,10 @@
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>33</v>
@@ -1546,7 +1546,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="12">
@@ -1566,10 +1566,10 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>33</v>
@@ -1674,10 +1674,10 @@
         <v>15</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>33</v>
@@ -1688,7 +1688,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1711,10 +1711,10 @@
         <v>15</v>
       </c>
       <c r="J3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>34</v>
@@ -1733,7 +1733,7 @@
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1855,10 +1855,10 @@
         <v>15</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>33</v>
@@ -1880,10 +1880,10 @@
         <v>23</v>
       </c>
       <c r="S2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="U2" s="7" t="s">
         <v>34</v>
@@ -1894,7 +1894,7 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1917,10 +1917,10 @@
         <v>15</v>
       </c>
       <c r="J3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>34</v>
@@ -1942,10 +1942,10 @@
         <v>14</v>
       </c>
       <c r="S3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="U3" s="7" t="s">
         <v>33</v>
@@ -1989,14 +1989,14 @@
     <row r="2" spans="1:4">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45302</v>
+        <v>45303</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45454</v>
+        <v>45455</v>
       </c>
       <c r="D2" s="8"/>
     </row>

</xml_diff>

<commit_message>
fix UI script ensinger
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A008A0-6B1D-4A8E-BE28-9EB1139251DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE95EE5-4457-461E-8C33-B57AAE6DE23B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA001" sheetId="4" r:id="rId1"/>
@@ -608,7 +608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -791,7 +791,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -907,7 +907,7 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
-        <v>5</v>
+        <v>300</v>
       </c>
       <c r="D3" s="4">
         <v>2</v>
@@ -996,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E9DDA8-B5FB-4116-AA3C-6DFE9FE54EE5}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
-        <v>201</v>
+        <v>400</v>
       </c>
       <c r="D3" s="4">
         <v>2</v>

</xml_diff>

<commit_message>
minor fix cannot read file excel
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20406"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE95EE5-4457-461E-8C33-B57AAE6DE23B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D22CF8F-EA7C-4CF5-9511-B477D804BDC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA001" sheetId="4" r:id="rId1"/>
@@ -185,9 +185,6 @@
     <t>142,11</t>
   </si>
   <si>
-    <t>183,38</t>
-  </si>
-  <si>
     <t>96,54</t>
   </si>
   <si>
@@ -228,6 +225,9 @@
   </si>
   <si>
     <t>stp-testing 4.stp</t>
+  </si>
+  <si>
+    <t>208,34</t>
   </si>
 </sst>
 </file>
@@ -645,7 +645,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -691,10 +691,10 @@
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>33</v>
@@ -708,7 +708,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -728,10 +728,10 @@
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>34</v>
@@ -745,7 +745,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -765,10 +765,10 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>33</v>
@@ -828,7 +828,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -880,10 +880,10 @@
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>33</v>
@@ -903,7 +903,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -923,10 +923,10 @@
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>34</v>
@@ -946,7 +946,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -966,10 +966,10 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>33</v>
@@ -996,7 +996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E9DDA8-B5FB-4116-AA3C-6DFE9FE54EE5}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -1034,7 +1034,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -1076,7 +1076,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>14</v>
@@ -1085,10 +1085,10 @@
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>33</v>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1118,7 +1118,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>24</v>
@@ -1127,10 +1127,10 @@
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>34</v>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1160,7 +1160,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>23</v>
@@ -1169,10 +1169,10 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>33</v>
@@ -1235,7 +1235,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -1290,17 +1290,17 @@
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>33</v>
       </c>
       <c r="L2" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45455</v>
+        <v>45461</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>16</v>
@@ -1312,12 +1312,12 @@
         <v>18</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1337,17 +1337,17 @@
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>34</v>
       </c>
       <c r="L3" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45455</v>
+        <v>45461</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>36</v>
@@ -1359,12 +1359,12 @@
         <v>18</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1384,17 +1384,17 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>33</v>
       </c>
       <c r="L4" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45455</v>
+        <v>45461</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>38</v>
@@ -1406,7 +1406,7 @@
         <v>18</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1455,7 +1455,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -1498,10 +1498,10 @@
         <v>4</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>33</v>
@@ -1512,7 +1512,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12">
@@ -1532,10 +1532,10 @@
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>33</v>
@@ -1546,7 +1546,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="12">
@@ -1566,10 +1566,10 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>33</v>
@@ -1625,7 +1625,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -1674,10 +1674,10 @@
         <v>15</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>33</v>
@@ -1688,7 +1688,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1711,10 +1711,10 @@
         <v>15</v>
       </c>
       <c r="J3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>34</v>
@@ -1732,9 +1732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247EA267-3747-4ADE-8941-713003159070}">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1779,7 +1777,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -1812,7 +1810,7 @@
         <v>29</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>30</v>
@@ -1855,16 +1853,16 @@
         <v>15</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>33</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="N2" s="4">
         <v>2</v>
@@ -1880,21 +1878,21 @@
         <v>23</v>
       </c>
       <c r="S2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="U2" s="7" t="s">
         <v>34</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1917,10 +1915,10 @@
         <v>15</v>
       </c>
       <c r="J3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>34</v>
@@ -1942,16 +1940,16 @@
         <v>14</v>
       </c>
       <c r="S3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="T3" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="U3" s="7" t="s">
         <v>33</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1989,14 +1987,14 @@
     <row r="2" spans="1:4">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45303</v>
+        <v>45309</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45455</v>
+        <v>45461</v>
       </c>
       <c r="D2" s="8"/>
     </row>

</xml_diff>

<commit_message>
minor fix change param
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20406"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637962C1-506A-4DBA-AAE8-545B6B0DAEAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776FAD37-CAA5-4342-BEEA-4BD7AF7CB0BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA001" sheetId="4" r:id="rId1"/>
@@ -845,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC3FC65-E1BB-4B27-9BAD-1FAD73694C2F}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -971,7 +971,7 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D3" s="4">
         <v>2</v>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="M2" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45449</v>
+        <v>45469</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>18</v>
@@ -1448,7 +1448,7 @@
       </c>
       <c r="M3" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45449</v>
+        <v>45469</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>45</v>
@@ -1500,7 +1500,7 @@
       </c>
       <c r="M4" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45449</v>
+        <v>45469</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>47</v>
@@ -1524,7 +1524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544CF78C-E801-4C61-A3AF-6B74429A6B71}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -2126,14 +2126,14 @@
     <row r="2" spans="1:4">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45297</v>
+        <v>45317</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45449</v>
+        <v>45469</v>
       </c>
       <c r="D2" s="8"/>
     </row>

</xml_diff>

<commit_message>
fix flow impact by shippingCost
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776FAD37-CAA5-4342-BEEA-4BD7AF7CB0BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C0F8C2-18CC-44B2-82C3-E8F0168CBE1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="79">
   <si>
     <t>fileName</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>Aluminum</t>
+  </si>
+  <si>
+    <t>shippingCost</t>
   </si>
 </sst>
 </file>
@@ -843,10 +846,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC3FC65-E1BB-4B27-9BAD-1FAD73694C2F}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -865,9 +868,10 @@
     <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.28515625" customWidth="1"/>
     <col min="16" max="16" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1">
+    <row r="1" spans="1:17" s="3" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -916,8 +920,11 @@
       <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
         <v>24</v>
       </c>
@@ -964,8 +971,11 @@
       <c r="P2" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Q2" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -1012,8 +1022,11 @@
       <c r="P3" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="Q3" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="4" t="s">
         <v>70</v>
       </c>
@@ -1059,6 +1072,9 @@
       </c>
       <c r="P4" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1396,7 +1412,7 @@
       </c>
       <c r="M2" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45469</v>
+        <v>45471</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>18</v>
@@ -1448,7 +1464,7 @@
       </c>
       <c r="M3" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45469</v>
+        <v>45471</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>45</v>
@@ -1500,7 +1516,7 @@
       </c>
       <c r="M4" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45469</v>
+        <v>45471</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>47</v>
@@ -2126,14 +2142,14 @@
     <row r="2" spans="1:4">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45317</v>
+        <v>45319</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45469</v>
+        <v>45471</v>
       </c>
       <c r="D2" s="8"/>
     </row>

</xml_diff>

<commit_message>
change name shipping option
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C0F8C2-18CC-44B2-82C3-E8F0168CBE1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24184E8-323C-4CCA-A389-F56C551DB34F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA001" sheetId="4" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>STANDARD</t>
   </si>
   <si>
-    <t>Standard shipping</t>
-  </si>
-  <si>
     <t>abc comment</t>
   </si>
   <si>
@@ -170,15 +167,9 @@
     <t>ECONOMY</t>
   </si>
   <si>
-    <t>Pickup at factory</t>
-  </si>
-  <si>
     <t>FAST</t>
   </si>
   <si>
-    <t>Special packaging / via freight forwarding</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -267,6 +258,15 @@
   </si>
   <si>
     <t>shippingCost</t>
+  </si>
+  <si>
+    <t>Package delivery (extra costs)</t>
+  </si>
+  <si>
+    <t>Pick-up at factory (no costs)</t>
+  </si>
+  <si>
+    <t>Freight delivery / sepcial packaging (extra costs)</t>
   </si>
 </sst>
 </file>
@@ -647,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:F21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -703,7 +703,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>12</v>
@@ -714,7 +714,7 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
@@ -727,7 +727,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>15</v>
@@ -739,24 +739,24 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -769,10 +769,10 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
@@ -781,24 +781,24 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -811,10 +811,10 @@
         <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="4">
         <v>7</v>
@@ -823,19 +823,19 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -848,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC3FC65-E1BB-4B27-9BAD-1FAD73694C2F}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -865,7 +865,7 @@
     <col min="10" max="10" width="22.140625" customWidth="1"/>
     <col min="11" max="12" width="18.85546875" customWidth="1"/>
     <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.42578125" customWidth="1"/>
     <col min="15" max="15" width="18.28515625" customWidth="1"/>
     <col min="16" max="16" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.28515625" customWidth="1"/>
@@ -906,7 +906,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>12</v>
@@ -915,18 +915,18 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
@@ -939,7 +939,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>15</v>
@@ -951,25 +951,25 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="N2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="Q2" s="4">
         <v>15</v>
@@ -977,7 +977,7 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -990,10 +990,10 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
@@ -1002,25 +1002,25 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q3" s="4">
         <v>6</v>
@@ -1028,7 +1028,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1041,10 +1041,10 @@
         <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="4">
         <v>7</v>
@@ -1053,25 +1053,25 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q4" s="4">
         <v>7</v>
@@ -1143,7 +1143,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>12</v>
@@ -1152,12 +1152,12 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
@@ -1170,7 +1170,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>15</v>
@@ -1179,30 +1179,30 @@
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1215,39 +1215,39 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1260,34 +1260,34 @@
         <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="4">
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1357,7 +1357,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>11</v>
@@ -1372,12 +1372,12 @@
         <v>14</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
@@ -1390,7 +1390,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>15</v>
@@ -1402,34 +1402,34 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M2" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45471</v>
+        <v>45476</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="O2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="Q2" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1442,10 +1442,10 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
@@ -1454,34 +1454,34 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M3" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45471</v>
+        <v>45476</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1494,10 +1494,10 @@
         <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="4">
         <v>7</v>
@@ -1506,29 +1506,29 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M4" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45471</v>
+        <v>45476</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1596,15 +1596,15 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
@@ -1617,7 +1617,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>15</v>
@@ -1626,24 +1626,24 @@
         <v>4</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12">
@@ -1656,10 +1656,10 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
@@ -1668,21 +1668,21 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="12">
@@ -1695,10 +1695,10 @@
         <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="4">
         <v>7</v>
@@ -1707,16 +1707,16 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1784,15 +1784,15 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
@@ -1805,7 +1805,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>15</v>
@@ -1817,21 +1817,21 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1844,10 +1844,10 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
@@ -1856,16 +1856,16 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1878,7 +1878,7 @@
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1942,42 +1942,42 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="V1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
@@ -1990,7 +1990,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>15</v>
@@ -2002,16 +2002,16 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="N2" s="4">
         <v>2</v>
@@ -2023,27 +2023,27 @@
         <v>6</v>
       </c>
       <c r="Q2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="7" t="s">
-        <v>40</v>
-      </c>
       <c r="V2" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -2056,10 +2056,10 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="4">
         <v>7</v>
@@ -2068,16 +2068,16 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N3" s="4">
         <v>1</v>
@@ -2089,22 +2089,22 @@
         <v>6</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="R3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="T3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="V3" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="V3" s="4" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2130,26 +2130,26 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45319</v>
+        <v>45325</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45471</v>
+        <v>45476</v>
       </c>
       <c r="D2" s="8"/>
     </row>

</xml_diff>

<commit_message>
minor fix buyer script auto
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24184E8-323C-4CCA-A389-F56C551DB34F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45BDB13-6C02-47BF-B132-CB54C7F5A79B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA001" sheetId="4" r:id="rId1"/>
@@ -194,9 +194,6 @@
     <t>SMALL_TOLERANCES</t>
   </si>
   <si>
-    <t>CALCULATION_ERROR</t>
-  </si>
-  <si>
     <t>stp-testing.stp</t>
   </si>
   <si>
@@ -267,6 +264,9 @@
   </si>
   <si>
     <t>Freight delivery / sepcial packaging (extra costs)</t>
+  </si>
+  <si>
+    <t>CANNOT_CALCULATE_PART</t>
   </si>
 </sst>
 </file>
@@ -647,7 +647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
@@ -739,7 +739,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -751,7 +751,7 @@
         <v>18</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -769,7 +769,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>26</v>
@@ -781,10 +781,10 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>39</v>
@@ -793,12 +793,12 @@
         <v>44</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -823,7 +823,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>38</v>
@@ -835,7 +835,7 @@
         <v>18</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -921,7 +921,7 @@
         <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -951,7 +951,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -963,7 +963,7 @@
         <v>18</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>21</v>
@@ -990,7 +990,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>26</v>
@@ -1002,10 +1002,10 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>39</v>
@@ -1014,7 +1014,7 @@
         <v>44</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>43</v>
@@ -1028,7 +1028,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1053,7 +1053,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>38</v>
@@ -1065,7 +1065,7 @@
         <v>45</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>43</v>
@@ -1182,7 +1182,7 @@
         <v>46</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1194,7 +1194,7 @@
         <v>18</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>21</v>
@@ -1227,7 +1227,7 @@
         <v>46</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>40</v>
@@ -1239,7 +1239,7 @@
         <v>44</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>43</v>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1272,7 +1272,7 @@
         <v>46</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>38</v>
@@ -1284,7 +1284,7 @@
         <v>45</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>43</v>
@@ -1402,7 +1402,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1412,19 +1412,19 @@
       </c>
       <c r="M2" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45476</v>
+        <v>45482</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1442,7 +1442,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>26</v>
@@ -1454,34 +1454,34 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>39</v>
       </c>
       <c r="M3" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45476</v>
+        <v>45482</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>44</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1506,7 +1506,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>38</v>
@@ -1516,19 +1516,19 @@
       </c>
       <c r="M4" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45476</v>
+        <v>45482</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>45</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1540,8 +1540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544CF78C-E801-4C61-A3AF-6B74429A6B71}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1629,7 +1629,7 @@
         <v>46</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12">
@@ -1668,7 +1668,7 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>38</v>
@@ -1677,7 +1677,7 @@
         <v>36</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1707,7 +1707,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>38</v>
@@ -1817,7 +1817,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1826,7 +1826,7 @@
         <v>36</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1856,7 +1856,7 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>40</v>
@@ -1865,7 +1865,7 @@
         <v>39</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1963,7 +1963,7 @@
         <v>33</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>34</v>
@@ -1990,7 +1990,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>15</v>
@@ -2002,16 +2002,16 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N2" s="4">
         <v>2</v>
@@ -2029,7 +2029,7 @@
         <v>25</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>38</v>
@@ -2038,7 +2038,7 @@
         <v>39</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -2068,16 +2068,16 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>39</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N3" s="4">
         <v>1</v>
@@ -2089,22 +2089,22 @@
         <v>6</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U3" s="7" t="s">
         <v>36</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2142,14 +2142,14 @@
     <row r="2" spans="1:4">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45325</v>
+        <v>45331</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45476</v>
+        <v>45482</v>
       </c>
       <c r="D2" s="8"/>
     </row>

</xml_diff>

<commit_message>
fix name shipping cost
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187C10E2-F3AA-4A22-A3AA-23EA73C505B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA99C14-BB0A-45DD-92ED-D090982529B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -263,10 +263,10 @@
     <t>Pick-up at factory (no costs)</t>
   </si>
   <si>
-    <t>Freight delivery / sepcial packaging (extra costs)</t>
-  </si>
-  <si>
     <t>CANNOT_CALCULATE_PART</t>
+  </si>
+  <si>
+    <t>Freight delivery / special packaging (extra costs)</t>
   </si>
 </sst>
 </file>
@@ -647,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -835,7 +835,7 @@
         <v>18</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1065,7 +1065,7 @@
         <v>45</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>43</v>
@@ -1284,7 +1284,7 @@
         <v>45</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>43</v>
@@ -1412,7 +1412,7 @@
       </c>
       <c r="M2" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45492</v>
+        <v>45493</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>18</v>
@@ -1464,7 +1464,7 @@
       </c>
       <c r="M3" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45492</v>
+        <v>45493</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>44</v>
@@ -1516,13 +1516,13 @@
       </c>
       <c r="M4" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45492</v>
+        <v>45493</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>45</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>19</v>
@@ -1677,7 +1677,7 @@
         <v>36</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -2142,14 +2142,14 @@
     <row r="2" spans="1:4">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45492</v>
+        <v>45493</v>
       </c>
       <c r="D2" s="8"/>
     </row>

</xml_diff>

<commit_message>
fix remove odd param
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844EA356-C4C1-4E57-9389-F9D44A57A7B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C54BF4-78AB-4A71-91CA-AF6E010ADCDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA001" sheetId="4" r:id="rId1"/>
@@ -23,14 +23,14 @@
     <sheet name="Calculate" sheetId="11" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'FPA008-009'!$A$1:$P$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'FPA008-009'!$A$1:$O$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="63">
   <si>
     <t>fileName</t>
   </si>
@@ -200,9 +200,6 @@
     <t>Plastic</t>
   </si>
   <si>
-    <t>compliances</t>
-  </si>
-  <si>
     <t>compliancesChanged</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
   </si>
   <si>
     <t>PC Optik (transparent)</t>
-  </si>
-  <si>
-    <t>Edit compliances</t>
   </si>
   <si>
     <t>stp-testing 3.stp</t>
@@ -603,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -616,16 +610,15 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" customWidth="1"/>
-    <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="27.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="27.85546875" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1">
+    <row r="1" spans="1:12" s="3" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -642,31 +635,28 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:12">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -680,30 +670,29 @@
       <c r="E2" s="4">
         <v>4</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4">
+      <c r="G2" s="4">
         <v>5</v>
       </c>
+      <c r="H2" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="I2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="K2" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="L2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="4" t="s">
         <v>34</v>
       </c>
@@ -717,32 +706,31 @@
       <c r="E3" s="4">
         <v>3</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="4">
+      <c r="G3" s="4">
         <v>7</v>
       </c>
+      <c r="H3" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="I3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="K3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="K3" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="L3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -754,26 +742,25 @@
       <c r="E4" s="4">
         <v>3</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="4">
+      <c r="G4" s="4">
         <v>7</v>
       </c>
+      <c r="H4" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="I4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="K4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="K4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="L4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -785,10 +772,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC3FC65-E1BB-4B27-9BAD-1FAD73694C2F}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -798,17 +785,16 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" customWidth="1"/>
-    <col min="10" max="11" width="18.85546875" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" customWidth="1"/>
-    <col min="15" max="15" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" customWidth="1"/>
+    <col min="9" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" customWidth="1"/>
+    <col min="14" max="14" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1">
+    <row r="1" spans="1:14" s="3" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -825,37 +811,34 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -869,36 +852,35 @@
       <c r="E2" s="4">
         <v>4</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4">
+      <c r="G2" s="4">
         <v>5</v>
       </c>
+      <c r="H2" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="I2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="K2" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="L2" s="4" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:14">
       <c r="A3" s="4" t="s">
         <v>34</v>
       </c>
@@ -912,38 +894,37 @@
       <c r="E3" s="4">
         <v>3</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="4">
+      <c r="G3" s="4">
         <v>7</v>
       </c>
+      <c r="H3" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="I3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="K3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="K3" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="L3" s="4" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -955,32 +936,31 @@
       <c r="E4" s="4">
         <v>3</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="4">
+      <c r="G4" s="4">
         <v>7</v>
       </c>
+      <c r="H4" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="I4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="K4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="K4" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="L4" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -991,10 +971,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E9DDA8-B5FB-4116-AA3C-6DFE9FE54EE5}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1004,17 +984,16 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1">
+    <row r="1" spans="1:13" s="3" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1031,34 +1010,31 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -1073,34 +1049,31 @@
         <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="4">
-        <v>5</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="M2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="N2" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
         <v>34</v>
       </c>
@@ -1115,36 +1088,33 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="4">
+      <c r="G3" s="4">
         <v>7</v>
       </c>
+      <c r="H3" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="I3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="K3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="K3" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="L3" s="4" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="N3" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1157,30 +1127,27 @@
         <v>3</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="4">
+      <c r="G4" s="4">
         <v>7</v>
       </c>
+      <c r="H4" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="I4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="K4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="K4" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="L4" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1191,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08C9849-CB54-465E-AADF-08DB0E1F7827}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1204,18 +1171,17 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="18.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1">
+    <row r="1" spans="1:15" s="3" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1232,40 +1198,37 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:15">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -1279,40 +1242,39 @@
       <c r="E2" s="4">
         <v>4</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4">
+      <c r="G2" s="4">
         <v>5</v>
       </c>
+      <c r="H2" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="I2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="5">
+      <c r="K2" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45493</v>
+        <v>45494</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="O2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:15">
       <c r="A3" s="4" t="s">
         <v>34</v>
       </c>
@@ -1326,42 +1288,41 @@
       <c r="E3" s="4">
         <v>3</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="4">
+      <c r="G3" s="4">
         <v>7</v>
       </c>
+      <c r="H3" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="I3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="K3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="5">
+      <c r="K3" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45493</v>
+        <v>45494</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="O3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:15">
       <c r="A4" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1373,36 +1334,35 @@
       <c r="E4" s="4">
         <v>3</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="4">
+      <c r="G4" s="4">
         <v>7</v>
       </c>
+      <c r="H4" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="I4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="K4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="5">
+      <c r="K4" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45493</v>
+        <v>45494</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1413,10 +1373,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{544CF78C-E801-4C61-A3AF-6B74429A6B71}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1426,16 +1386,15 @@
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1452,28 +1411,25 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:11">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -1487,27 +1443,26 @@
       <c r="E2" s="4">
         <v>3</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4">
+      <c r="G2" s="4">
         <v>4</v>
       </c>
+      <c r="H2" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="I2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:11">
       <c r="A3" s="4" t="s">
         <v>46</v>
       </c>
@@ -1521,29 +1476,28 @@
       <c r="E3" s="12">
         <v>3</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="4">
+      <c r="G3" s="4">
         <v>7</v>
       </c>
+      <c r="H3" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="I3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="K3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:11">
       <c r="A4" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="12">
@@ -1555,23 +1509,22 @@
       <c r="E4" s="12">
         <v>3</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="4">
+      <c r="G4" s="4">
         <v>7</v>
       </c>
+      <c r="H4" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="I4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="K4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1582,10 +1535,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504AB99D-61BC-4A19-95BC-D98B671BEA2F}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1595,17 +1548,16 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1622,31 +1574,28 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:12">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -1660,30 +1609,29 @@
       <c r="E2" s="4">
         <v>3</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4">
+      <c r="G2" s="4">
         <v>4</v>
       </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I2" s="4" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="L2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:12">
       <c r="A3" s="4" t="s">
         <v>34</v>
       </c>
@@ -1697,26 +1645,25 @@
       <c r="E3" s="4">
         <v>3</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="4">
+      <c r="G3" s="4">
         <v>7</v>
       </c>
+      <c r="H3" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I3" s="4" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="L3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1727,10 +1674,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247EA267-3747-4ADE-8941-713003159070}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1740,26 +1687,25 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1"/>
-    <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="12" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
-    <col min="14" max="14" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="33" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" customWidth="1"/>
+    <col min="13" max="13" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="3" customFormat="1">
+    <row r="1" spans="1:21" s="3" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1776,58 +1722,55 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:21">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -1841,55 +1784,54 @@
       <c r="E2" s="4">
         <v>3</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4">
+      <c r="G2" s="4">
         <v>4</v>
       </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I2" s="4" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="L2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>51</v>
       </c>
+      <c r="M2" s="4">
+        <v>2</v>
+      </c>
       <c r="N2" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O2" s="4">
-        <v>5</v>
-      </c>
-      <c r="P2" s="4">
         <v>6</v>
       </c>
-      <c r="Q2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="R2" s="4" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="U2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="T2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:21">
       <c r="A3" s="4" t="s">
         <v>34</v>
       </c>
@@ -1903,51 +1845,50 @@
       <c r="E3" s="4">
         <v>3</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="4">
+      <c r="G3" s="4">
         <v>7</v>
       </c>
+      <c r="H3" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="I3" s="4" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="L3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="M3" s="4">
+        <v>1</v>
+      </c>
       <c r="N3" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="O3" s="4">
-        <v>5</v>
-      </c>
-      <c r="P3" s="4">
         <v>6</v>
       </c>
-      <c r="Q3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="R3" s="4" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="U3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="U3" s="4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1986,14 +1927,14 @@
     <row r="2" spans="1:4">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45342</v>
+        <v>45343</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45493</v>
+        <v>45494</v>
       </c>
       <c r="D2" s="8"/>
     </row>

</xml_diff>

<commit_message>
change name file part
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20407"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA99C14-BB0A-45DD-92ED-D090982529B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5FDDD1-ED25-4649-9F72-7E7CB823190E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -158,9 +158,6 @@
     <t>Glass bead blasting</t>
   </si>
   <si>
-    <t>stp-testing 2.stp</t>
-  </si>
-  <si>
     <t>58,04</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
     <t>Date M added</t>
   </si>
   <si>
-    <t>step-testing 2.step</t>
-  </si>
-  <si>
     <t>codeManual</t>
   </si>
   <si>
@@ -267,6 +261,12 @@
   </si>
   <si>
     <t>Freight delivery / special packaging (extra costs)</t>
+  </si>
+  <si>
+    <t>stp-testing-2.stp</t>
+  </si>
+  <si>
+    <t>step-testing-2.step</t>
   </si>
 </sst>
 </file>
@@ -647,9 +647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -739,7 +737,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -751,12 +749,12 @@
         <v>18</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="4" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -769,7 +767,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>26</v>
@@ -781,24 +779,24 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>39</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -823,7 +821,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>38</v>
@@ -835,7 +833,7 @@
         <v>18</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC3FC65-E1BB-4B27-9BAD-1FAD73694C2F}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -921,7 +919,7 @@
         <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -951,7 +949,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -963,7 +961,7 @@
         <v>18</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>21</v>
@@ -977,7 +975,7 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="4" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -990,7 +988,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>26</v>
@@ -1002,22 +1000,22 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>39</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>19</v>
@@ -1028,7 +1026,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1053,7 +1051,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>38</v>
@@ -1062,13 +1060,13 @@
         <v>36</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>19</v>
@@ -1179,10 +1177,10 @@
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1194,7 +1192,7 @@
         <v>18</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>21</v>
@@ -1202,7 +1200,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="4" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1224,10 +1222,10 @@
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>40</v>
@@ -1236,18 +1234,18 @@
         <v>39</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1269,10 +1267,10 @@
         <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>38</v>
@@ -1281,13 +1279,13 @@
         <v>36</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1299,7 +1297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08C9849-CB54-465E-AADF-08DB0E1F7827}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
@@ -1402,7 +1400,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1412,24 +1410,24 @@
       </c>
       <c r="M2" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45493</v>
+        <v>45514</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="4" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1442,7 +1440,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>26</v>
@@ -1454,34 +1452,34 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>39</v>
       </c>
       <c r="M3" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45493</v>
+        <v>45514</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
@@ -1506,7 +1504,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>38</v>
@@ -1516,19 +1514,19 @@
       </c>
       <c r="M4" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45493</v>
+        <v>45514</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1541,7 +1539,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1599,7 +1597,7 @@
         <v>27</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1626,10 +1624,10 @@
         <v>4</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1638,12 +1636,12 @@
         <v>36</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12">
@@ -1668,7 +1666,7 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>38</v>
@@ -1677,12 +1675,12 @@
         <v>36</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="12">
@@ -1707,7 +1705,7 @@
         <v>16</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>38</v>
@@ -1716,7 +1714,7 @@
         <v>36</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1817,7 +1815,7 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>17</v>
@@ -1826,12 +1824,12 @@
         <v>36</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1856,7 +1854,7 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>40</v>
@@ -1865,7 +1863,7 @@
         <v>39</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1877,7 +1875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247EA267-3747-4ADE-8941-713003159070}">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
@@ -1963,7 +1961,7 @@
         <v>33</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>34</v>
@@ -1990,7 +1988,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>15</v>
@@ -2002,16 +2000,16 @@
         <v>16</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N2" s="4">
         <v>2</v>
@@ -2029,7 +2027,7 @@
         <v>25</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>38</v>
@@ -2038,12 +2036,12 @@
         <v>39</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="4" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -2068,16 +2066,16 @@
         <v>16</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>39</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N3" s="4">
         <v>1</v>
@@ -2089,22 +2087,22 @@
         <v>6</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="R3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="U3" s="7" t="s">
         <v>36</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2130,26 +2128,26 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45342</v>
+        <v>45361</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45493</v>
+        <v>45514</v>
       </c>
       <c r="D2" s="8"/>
     </row>

</xml_diff>

<commit_message>
fix issue auto script
</commit_message>
<xml_diff>
--- a/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
+++ b/Data/Milled Or Turned Parts/Order/Order Information (MTP).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Milled Or Turned Parts\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16421619-F9E9-4C8B-8C0E-AD49418EDD68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A1DAFC-4A70-4A66-B751-15CFEF2E1F55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -846,7 +846,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC3FC65-E1BB-4B27-9BAD-1FAD73694C2F}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -926,7 +928,7 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4">
-        <v>70</v>
+        <v>300</v>
       </c>
       <c r="D2" s="4">
         <v>3</v>
@@ -1408,7 +1410,7 @@
       </c>
       <c r="M2" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>18</v>
@@ -1460,7 +1462,7 @@
       </c>
       <c r="M3" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>43</v>
@@ -1512,7 +1514,7 @@
       </c>
       <c r="M4" s="5">
         <f ca="1">Calculate!$C$2</f>
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>44</v>
@@ -2138,14 +2140,14 @@
     <row r="2" spans="1:4">
       <c r="A2" s="10">
         <f ca="1">TODAY()</f>
-        <v>45361</v>
+        <v>45365</v>
       </c>
       <c r="B2" s="9">
         <v>5</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45514</v>
+        <v>45518</v>
       </c>
       <c r="D2" s="8"/>
     </row>

</xml_diff>